<commit_message>
Test cases updated with wait utility and description added for all test cases.
</commit_message>
<xml_diff>
--- a/QaLegend/src/main/resources/ExcelFiles/TestData.xlsx
+++ b/QaLegend/src/main/resources/ExcelFiles/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Welcome Mercy,</t>
   </si>
   <si>
-    <t>Test@gmail.com</t>
-  </si>
-  <si>
     <t>We have e-mailed your password reset link!</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>Showing 1 to 3 of 3 entries</t>
+  </si>
+  <si>
+    <t>test1238@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,10 +473,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +581,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>